<commit_message>
Fix : more condition on KRS import
</commit_message>
<xml_diff>
--- a/public/template/template_import_krs.xlsx
+++ b/public/template/template_import_krs.xlsx
@@ -806,17 +806,17 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Rockwell"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Rockwell"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="37">
@@ -1662,7 +1662,7 @@
   <sheetPr/>
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K27" sqref="K27:K49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Feat : create new KRS
</commit_message>
<xml_diff>
--- a/public/template/template_import_krs.xlsx
+++ b/public/template/template_import_krs.xlsx
@@ -787,21 +787,14 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <b/>
+      <sz val="9"/>
+      <name val="Rockwell"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Rockwell"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
       <name val="Rockwell"/>
       <charset val="134"/>
     </font>
@@ -812,6 +805,13 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>

</xml_diff>

<commit_message>
Feat : KRS Export all
</commit_message>
<xml_diff>
--- a/public/template/template_import_krs.xlsx
+++ b/public/template/template_import_krs.xlsx
@@ -787,6 +787,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="9"/>
       <name val="Rockwell"/>
@@ -805,13 +812,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1663,7 +1663,7 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27:K49"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>